<commit_message>
added monthly/yearly BEV brand charts
</commit_message>
<xml_diff>
--- a/data/data_raw/eurostat/AT_gas_NRG_CB_GASM.xlsx
+++ b/data/data_raw/eurostat/AT_gas_NRG_CB_GASM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:HB33"/>
+  <dimension ref="A1:HC33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1477,6 +1477,11 @@
       <c r="HB1" s="1" t="inlineStr">
         <is>
           <t>2024-12</t>
+        </is>
+      </c>
+      <c r="HC1" s="1" t="inlineStr">
+        <is>
+          <t>2025-01</t>
         </is>
       </c>
     </row>
@@ -1975,8 +1980,9 @@
         <v>43.094</v>
       </c>
       <c r="HB2" t="n">
-        <v>44.531</v>
-      </c>
+        <v>45.573</v>
+      </c>
+      <c r="HC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2617,8 +2623,9 @@
         <v>1686.686</v>
       </c>
       <c r="HB3" t="n">
-        <v>1742.909</v>
-      </c>
+        <v>1783.681</v>
+      </c>
+      <c r="HC3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2971,8 +2978,9 @@
         <v>0.835</v>
       </c>
       <c r="HB4" t="n">
-        <v>0.863</v>
-      </c>
+        <v>0.95</v>
+      </c>
+      <c r="HC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -3325,8 +3333,9 @@
         <v>32.684</v>
       </c>
       <c r="HB5" t="n">
-        <v>33.773</v>
-      </c>
+        <v>37.184</v>
+      </c>
+      <c r="HC5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -3823,8 +3832,9 @@
         <v>925.204</v>
       </c>
       <c r="HB6" t="n">
-        <v>1149.566</v>
-      </c>
+        <v>1143.843</v>
+      </c>
+      <c r="HC6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -4465,8 +4475,9 @@
         <v>36211.891</v>
       </c>
       <c r="HB7" t="n">
-        <v>44993.267</v>
-      </c>
+        <v>44769.235</v>
+      </c>
+      <c r="HC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -4963,8 +4974,9 @@
         <v>534.159</v>
       </c>
       <c r="HB8" t="n">
-        <v>1202.223</v>
-      </c>
+        <v>1211.748</v>
+      </c>
+      <c r="HC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -5605,8 +5617,9 @@
         <v>20906.649</v>
       </c>
       <c r="HB9" t="n">
-        <v>47054.204</v>
-      </c>
+        <v>47427.007</v>
+      </c>
+      <c r="HC9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -5881,6 +5894,7 @@
       <c r="HB10" t="n">
         <v>0</v>
       </c>
+      <c r="HC10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -6155,6 +6169,7 @@
       <c r="HB11" t="n">
         <v>0</v>
       </c>
+      <c r="HC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -6651,8 +6666,9 @@
         <v>-499.504</v>
       </c>
       <c r="HB12" t="n">
-        <v>-1012.998</v>
-      </c>
+        <v>-1014.248</v>
+      </c>
+      <c r="HC12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -7293,8 +7309,9 @@
         <v>-19550.269</v>
       </c>
       <c r="HB13" t="n">
-        <v>-39648.053</v>
-      </c>
+        <v>-39697.01</v>
+      </c>
+      <c r="HC13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -7625,6 +7642,7 @@
       <c r="HB14" t="n">
         <v>0</v>
       </c>
+      <c r="HC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -7955,6 +7973,7 @@
       <c r="HB15" t="n">
         <v>0</v>
       </c>
+      <c r="HC15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -8451,8 +8470,9 @@
         <v>956.178</v>
       </c>
       <c r="HB16" t="n">
-        <v>0</v>
-      </c>
+        <v>1009.993</v>
+      </c>
+      <c r="HC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -8973,8 +8993,9 @@
         <v>37424.172</v>
       </c>
       <c r="HB17" t="n">
-        <v>0</v>
-      </c>
+        <v>39530.463</v>
+      </c>
+      <c r="HC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -9471,8 +9492,9 @@
         <v>950.345</v>
       </c>
       <c r="HB18" t="n">
-        <v>1005.735</v>
-      </c>
+        <v>992.866</v>
+      </c>
+      <c r="HC18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -10113,8 +10135,9 @@
         <v>37195.881</v>
       </c>
       <c r="HB19" t="n">
-        <v>39363.798</v>
-      </c>
+        <v>38860.103</v>
+      </c>
+      <c r="HC19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -10611,8 +10634,9 @@
         <v>307.55</v>
       </c>
       <c r="HB20" t="n">
-        <v>0</v>
-      </c>
+        <v>300.675</v>
+      </c>
+      <c r="HC20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -11181,8 +11205,9 @@
         <v>12037.318</v>
       </c>
       <c r="HB21" t="n">
-        <v>0</v>
-      </c>
+        <v>11768.219</v>
+      </c>
+      <c r="HC21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -11679,8 +11704,9 @@
         <v>10.462</v>
       </c>
       <c r="HB22" t="n">
-        <v>0</v>
-      </c>
+        <v>11.18</v>
+      </c>
+      <c r="HC22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -12321,8 +12347,9 @@
         <v>409.493</v>
       </c>
       <c r="HB23" t="n">
-        <v>0</v>
-      </c>
+        <v>437.571</v>
+      </c>
+      <c r="HC23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -12653,6 +12680,7 @@
       <c r="HB24" t="n">
         <v>0</v>
       </c>
+      <c r="HC24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -12983,6 +13011,7 @@
       <c r="HB25" t="n">
         <v>0</v>
       </c>
+      <c r="HC25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -13313,6 +13342,7 @@
       <c r="HB26" t="n">
         <v>0</v>
       </c>
+      <c r="HC26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -13643,6 +13673,7 @@
       <c r="HB27" t="n">
         <v>0</v>
       </c>
+      <c r="HC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -13878,9 +13909,8 @@
       <c r="GY28" t="inlineStr"/>
       <c r="GZ28" t="inlineStr"/>
       <c r="HA28" t="inlineStr"/>
-      <c r="HB28" t="n">
-        <v>0</v>
-      </c>
+      <c r="HB28" t="inlineStr"/>
+      <c r="HC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -14116,9 +14146,8 @@
       <c r="GY29" t="inlineStr"/>
       <c r="GZ29" t="inlineStr"/>
       <c r="HA29" t="inlineStr"/>
-      <c r="HB29" t="n">
-        <v>0</v>
-      </c>
+      <c r="HB29" t="inlineStr"/>
+      <c r="HC29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -14385,8 +14414,9 @@
         <v>199.507</v>
       </c>
       <c r="HB30" t="n">
-        <v>0</v>
-      </c>
+        <v>316.012</v>
+      </c>
+      <c r="HC30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -14653,8 +14683,9 @@
         <v>7808.59</v>
       </c>
       <c r="HB31" t="n">
-        <v>0</v>
-      </c>
+        <v>12368.482</v>
+      </c>
+      <c r="HC31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -15007,8 +15038,9 @@
         <v>-5.833</v>
       </c>
       <c r="HB32" t="n">
-        <v>1005.735</v>
-      </c>
+        <v>-17.127</v>
+      </c>
+      <c r="HC32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -15361,8 +15393,9 @@
         <v>-228.291</v>
       </c>
       <c r="HB33" t="n">
-        <v>39363.798</v>
-      </c>
+        <v>-670.36</v>
+      </c>
+      <c r="HC33" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>